<commit_message>
Add Purchase service, fix inventory update, and improve file handling
- Implemented the Purchase service
- Fixed inventory update issues
- Resolved file path issue in inventory service
- Added support for posting multiple products
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -43,40 +43,31 @@
     <t>Widget B</t>
   </si>
   <si>
-    <t>A Dazzling widget</t>
-  </si>
-  <si>
     <t>0ea6502c-d8c3-4381-b5d9-96fa2c76edf4</t>
   </si>
   <si>
-    <t>1f90943c-ba00-45b6-9356-d313542d8cfa</t>
-  </si>
-  <si>
     <t>Widget C</t>
   </si>
   <si>
-    <t>A Premium widget</t>
-  </si>
-  <si>
-    <t>e4815cc3-2fd5-4a46-a4b6-8d3c5bf03dd8</t>
-  </si>
-  <si>
     <t>Widget D</t>
   </si>
   <si>
-    <t>A Cool widget</t>
-  </si>
-  <si>
-    <t>6c9a9187-a50d-49da-bf2f-a1eaa677ca21</t>
-  </si>
-  <si>
-    <t>Test Product</t>
-  </si>
-  <si>
-    <t>A test description</t>
-  </si>
-  <si>
-    <t/>
+    <t>20</t>
+  </si>
+  <si>
+    <t>23dff0ee-e4b4-4fdf-a9ed-52c93a98eaef</t>
+  </si>
+  <si>
+    <t>cce54d6e-76c7-46ea-96ba-30b6be39eb8f</t>
+  </si>
+  <si>
+    <t>A good-qauality widget</t>
+  </si>
+  <si>
+    <t>A dazzling widget</t>
+  </si>
+  <si>
+    <t>A premium widget</t>
   </si>
 </sst>
 </file>
@@ -391,7 +382,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -415,7 +406,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -427,7 +418,7 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -438,30 +429,30 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>180</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="E4">
         <v>30</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -469,33 +460,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix - Report file path  Add - purchase service tests
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -31,43 +31,46 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Widget A</t>
-  </si>
-  <si>
-    <t>A high-quality widget</t>
-  </si>
-  <si>
-    <t>def0168e-bae7-4dbd-b4f0-e573eb1208f5</t>
-  </si>
-  <si>
-    <t>Widget B</t>
-  </si>
-  <si>
-    <t>0ea6502c-d8c3-4381-b5d9-96fa2c76edf4</t>
+    <t>fa694862-f183-4200-8896-4caf5cec47d3</t>
+  </si>
+  <si>
+    <t>Dropdown A</t>
+  </si>
+  <si>
+    <t>A high-qauality dropdown</t>
+  </si>
+  <si>
+    <t>7a95839e-7075-40c8-9c46-a5990084fb46</t>
+  </si>
+  <si>
+    <t>Dropdown B</t>
+  </si>
+  <si>
+    <t>ba6f6cb7-a21f-4898-a1df-2731b4239fcb</t>
+  </si>
+  <si>
+    <t>Widget D</t>
+  </si>
+  <si>
+    <t>A good-qauality widget</t>
+  </si>
+  <si>
+    <t>e0f79033-b1c3-437d-9b29-95057c11baa2</t>
   </si>
   <si>
     <t>Widget C</t>
   </si>
   <si>
-    <t>Widget D</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>23dff0ee-e4b4-4fdf-a9ed-52c93a98eaef</t>
-  </si>
-  <si>
-    <t>cce54d6e-76c7-46ea-96ba-30b6be39eb8f</t>
-  </si>
-  <si>
-    <t>A good-qauality widget</t>
-  </si>
-  <si>
-    <t>A dazzling widget</t>
-  </si>
-  <si>
     <t>A premium widget</t>
+  </si>
+  <si>
+    <t>9a3c15bf-2cd8-4c06-9c43-a1aaf680c68a</t>
+  </si>
+  <si>
+    <t>Widget E</t>
+  </si>
+  <si>
+    <t>A heavily used widget</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -406,79 +409,90 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
+      <c r="D3">
+        <v>15</v>
       </c>
       <c r="E3">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>35</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
         <v>25</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{9d258917-277f-42cd-a3cd-14c4e9ee58bc}" enabled="1" method="Standard" siteId="{38ae3bcd-9579-4fd4-adda-b42e1495d55a}" contentBits="0" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Fix - Inventory service tests
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -435,10 +435,10 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5">

</xml_diff>

<commit_message>
Fix - Purchase service tests
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -2,9 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
-  <workbookPr filterPrivacy="true"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F039C4B-D61B-4F70-BF2F-065F1888926F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -53,31 +54,13 @@
   </si>
   <si>
     <t>A good-qauality widget</t>
-  </si>
-  <si>
-    <t>e0f79033-b1c3-437d-9b29-95057c11baa2</t>
-  </si>
-  <si>
-    <t>Widget C</t>
-  </si>
-  <si>
-    <t>A premium widget</t>
-  </si>
-  <si>
-    <t>9a3c15bf-2cd8-4c06-9c43-a1aaf680c68a</t>
-  </si>
-  <si>
-    <t>Widget E</t>
-  </si>
-  <si>
-    <t>A heavily used widget</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,7 +95,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -125,7 +108,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -384,13 +367,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -424,7 +407,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -438,10 +421,10 @@
         <v>50</v>
       </c>
       <c r="E3">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -456,40 +439,6 @@
       </c>
       <c r="E4">
         <v>24</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>35</v>
-      </c>
-      <c r="E5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6">
-        <v>25</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added CORS in middlewares
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -2,10 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F039C4B-D61B-4F70-BF2F-065F1888926F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="true"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -54,13 +53,31 @@
   </si>
   <si>
     <t>A good-qauality widget</t>
+  </si>
+  <si>
+    <t>d7a56655-9107-4f4f-a66c-c9fb772211f2</t>
+  </si>
+  <si>
+    <t>Widget C</t>
+  </si>
+  <si>
+    <t>A premium widget</t>
+  </si>
+  <si>
+    <t>a215890f-bdff-4826-9f09-04ca812c69f6</t>
+  </si>
+  <si>
+    <t>Widget E</t>
+  </si>
+  <si>
+    <t>A heavily used widget</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,7 +112,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -108,7 +125,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -367,13 +384,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,7 +407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -404,10 +421,10 @@
         <v>15</v>
       </c>
       <c r="E2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -424,7 +441,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -439,6 +456,40 @@
       </c>
       <c r="E4">
         <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add EDIT, DEDUCT, REPORT features
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -71,6 +71,42 @@
   </si>
   <si>
     <t>A heavily used widget</t>
+  </si>
+  <si>
+    <t>64000e64-3d2e-4d57-a1a8-a955d7520478</t>
+  </si>
+  <si>
+    <t>Widget A</t>
+  </si>
+  <si>
+    <t>A Premium Widget</t>
+  </si>
+  <si>
+    <t>eb3e53df-7935-439d-8c7b-04d2047f68a8</t>
+  </si>
+  <si>
+    <t>WidgetB</t>
+  </si>
+  <si>
+    <t>A low grade Widget</t>
+  </si>
+  <si>
+    <t>c7b65e32-1a9f-40f1-9b04-89b69248c9a1</t>
+  </si>
+  <si>
+    <t>Dropdown C</t>
+  </si>
+  <si>
+    <t>A good looking dropdown</t>
+  </si>
+  <si>
+    <t>5bf4ec97-f9a9-46c1-8f98-b169c5c6686d</t>
+  </si>
+  <si>
+    <t>Dropdown D</t>
+  </si>
+  <si>
+    <t>A premium dropdown</t>
   </si>
 </sst>
 </file>
@@ -382,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -421,7 +457,7 @@
         <v>15</v>
       </c>
       <c r="E2">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -438,7 +474,7 @@
         <v>50</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -458,7 +494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -475,7 +511,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -490,6 +526,74 @@
       </c>
       <c r="E6">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>